<commit_message>
add feature user can custom node
</commit_message>
<xml_diff>
--- a/notebook/exper_id3_selectedStats_2hops.xlsx
+++ b/notebook/exper_id3_selectedStats_2hops.xlsx
@@ -111,19 +111,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -159,15 +153,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -484,14 +475,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="43.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="43.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="28.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -589,7 +580,7 @@
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>9000</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -620,14 +611,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="45.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="39.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="45.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -769,7 +760,7 @@
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>9000</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -800,14 +791,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -953,7 +944,7 @@
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>9000</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -984,14 +975,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="34.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="34.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1181,7 +1172,7 @@
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>9000</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1212,17 +1203,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="29.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="26.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="29.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="26.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1259,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1279,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1310,7 +1301,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1332,7 +1323,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1363,7 +1354,7 @@
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>90</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1394,14 +1385,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1593,7 +1584,7 @@
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>9000</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1626,14 +1617,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="30.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="30.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1781,7 +1772,7 @@
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>9000</v>
       </c>
       <c r="D7" s="1" t="s">

</xml_diff>